<commit_message>
Update WebUI and pom.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/ClientsDataExcel.xlsx
+++ b/src/test/resources/ClientsDataExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJavaFramework\projectTestNG\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumTestNGParallel\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D44C665-F5D2-4EDA-A072-7D93D420D62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910AF921-8789-4892-AE63-F78E4D358D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
@@ -103,10 +103,10 @@
     <t>Team Leader 01</t>
   </si>
   <si>
-    <t>Anh Tester Com 03</t>
-  </si>
-  <si>
-    <t>Anh Tester Com 04</t>
+    <t>Anh Tester Com 05</t>
+  </si>
+  <si>
+    <t>Anh Tester Com 06</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>14</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>24</v>

</xml_diff>